<commit_message>
Add Results and Ensemble Models
</commit_message>
<xml_diff>
--- a/Datasets/tobacco_data.xlsx
+++ b/Datasets/tobacco_data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="4" documentId="8_{85CDB0F4-28AD-454E-89EF-17679DA70D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4D7D71C-731D-4C29-BD95-0BF8FBB79CEA}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{6049EA67-DD7E-451A-8247-36CF987127C2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6049EA67-DD7E-451A-8247-36CF987127C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -734,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE6FBDBE-EF5D-4EFE-AAC8-A0D62986DC39}">
   <dimension ref="A1:M109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="E109" sqref="E109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>